<commit_message>
Subiendo mi proyecto a GitHub
</commit_message>
<xml_diff>
--- a/texto/text_report.xlsx
+++ b/texto/text_report.xlsx
@@ -1,37 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\OneDrive\Escritorio\Implementacion_Alerta_temprana\reporte\texto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EAD5BB-03D1-412B-BBA6-AC22752ECA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Semana</t>
+  </si>
+  <si>
+    <t>Parrafo1</t>
+  </si>
+  <si>
+    <t>Parrafo2</t>
+  </si>
+  <si>
+    <t>Parrafo3</t>
+  </si>
+  <si>
+    <t>Cambio_porc_ult</t>
+  </si>
+  <si>
+    <t>Cambio_porc_medio_3</t>
+  </si>
+  <si>
+    <t>34.7%</t>
+  </si>
+  <si>
+    <t>-23.2%</t>
+  </si>
+  <si>
+    <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 24px; text-align: justify;'&gt;En la semana epidemiológica 31 del año 2024, el número acumulado de casos de dengue en Perú asciende a 259,357. Los departamentos de Lima, La Libertad y Piura han registrado la mayor cantidad de casos acumulados hasta la fecha (Tabla N°1). La variación porcentual en la última semana muestra un cambio del 34.7%. Sin embargo, esta tendencia podría fluctuar en las semanas siguientes debido a la actualización de datos. Se ha observado un patrón de descenso en las semanas anteriores, con variaciones porcentuales de -17.2%, -13.6% y -23.2% (Gráfico N°1). Los departamentos que han experimentado el mayor cambio porcentual en la última semana son Callao, Ica y Madre de Dios. Además, los departamentos de Madre de Dios, Huanuco y Amazonas han mostrado el mayor cambio porcentual promedio en las tres semanas previas a la última (Tabla N°1).&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 24px; text-align: justify;'&gt;A nivel departamental, se ha notificado un primer caso de dengue en la última semana después de 5 años sin casos de dengue, lo que eleva a uno el número de departamentos que han notificado por primera vez después de ese período. A su vez, a nivel distrital, en la última semana, dos distritos han notificado el primer caso de dengue después de 5 años de no reportar casos, lo que elevó a 95 los distritos que han notificado su primer caso después de 5 años de dengue este año (Tabla N°1).&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 24px; text-align: justify;'&gt;Según los datos históricos de años sin brotes, se observa un aumento superior a lo esperado en 22 distritos, que se encuentran en condición de alarma. Aunque este crecimiento es significativo, no alcanza aún el nivel de alarma. En efecto, 106 distritos están en alerta, lo que sugiere un crecimiento notable en el número de casos (Gráfico N°2).&lt;/div&gt;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +93,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,87 +417,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Ano</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Semana</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Parrafo1</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Parrafo2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Parrafo3</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Cambio_porc_ult</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Cambio_porc_medio_3</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>2024</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>31</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 30px; text-align: justify;'&gt;En la semana epidemiológica 31 del año 2024, el número acumulado de casos de dengue en Perú asciende a 259,357. Los departamentos de Lima, La Libertad y Piura han registrado la mayor cantidad de casos acumulados hasta la fecha (Tabla N°1). La variación porcentual en la última semana muestra un cambio del 34,7%. Sin embargo, esta tendencia podría fluctuar en las semanas siguientes debido a la actualización de datos. Se ha observado un patrón de descenso en las semanas anteriores, con variaciones porcentuales de -17,2%, -13,6% y -23,2% (Gráfico N°1). Los departamentos que han experimentado el mayor cambio porcentual en la última semana son Callao, Ica y Madre de Dios. Además, los departamentos de Madre de Dios, Huanuco y Amazonas han mostrado el mayor cambio porcentual promedio en las tres semanas previas a la última (Tabla N°1).&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 30px; text-align: justify;'&gt;A nivel departamental, se ha notificado un primer caso de dengue en la última semana luego de una ausencia de 5 años de casos de dengue. Esto eleva a uno el número de departamentos que han notificado por primera vez después de 5 años. A su vez, a nivel distrital, en la última semana, dos distritos han notificado el primer caso de dengue luego de una ausencia de 5 años de reportes de casos, lo que elevó a 95 los distritos que han notificado su primer caso después de 5 años de dengue este año (Tabla N°1).&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>&lt;div tabindex='0' id='htmlContent' style='font-family: Arial; font-size: 30px; text-align: justify;'&gt;Según los datos históricos de años sin brotes, se observa un aumento superior a lo esperado en 22 distritos, que se encuentran en condición de alarma. Aunque, 106 distritos están en alerta, lo que sugiere un crecimiento significativo en el número de casos, no alcanzan aún los niveles de alarma (Gráfico N°2).&lt;/div&gt;</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>34.7%</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-23.2%</t>
-        </is>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>